<commit_message>
Added Label_Template to print on.
</commit_message>
<xml_diff>
--- a/MachineNames.xlsx
+++ b/MachineNames.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Limerick\Documentation\NUC_placements\Rev3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B902D3-F1D9-4F64-9CAA-4A978010BB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242542A5-C9A8-463F-8DB4-244C0ED970B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32385" yWindow="-2070" windowWidth="24045" windowHeight="15570" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="420" windowWidth="16800" windowHeight="14880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="125">
   <si>
     <t>VerticalBoards</t>
   </si>
@@ -402,6 +411,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Annunciator</t>
   </si>
 </sst>
 </file>
@@ -484,19 +496,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -812,7 +852,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{131A950B-39F6-44D9-9B29-4CDDD64DEB4D}" name="Table1" displayName="Table1" ref="A1:B16" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{131A950B-39F6-44D9-9B29-4CDDD64DEB4D}" name="Table1" displayName="Table1" ref="A1:B16" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="A1:B16" xr:uid="{131A950B-39F6-44D9-9B29-4CDDD64DEB4D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0982C118-CA94-4BF0-ACE3-0E93F55B7C93}" name="VerticalBoards"/>
@@ -823,7 +863,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A3D4546A-10D1-4880-B38E-6E6DA3DE4C8A}" name="Table2" displayName="Table2" ref="A18:B27" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A3D4546A-10D1-4880-B38E-6E6DA3DE4C8A}" name="Table2" displayName="Table2" ref="A18:B27" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A18:B27" xr:uid="{A3D4546A-10D1-4880-B38E-6E6DA3DE4C8A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{B7BDDF55-873E-43DF-AF8A-9185905BE765}" name="BenchBoards"/>
@@ -834,10 +874,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{51C8EE75-88EB-44C3-B3DF-8EDD52F15786}" name="Table3" displayName="Table3" ref="A29:B38" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{51C8EE75-88EB-44C3-B3DF-8EDD52F15786}" name="Table3" displayName="Table3" ref="A29:B38" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="A29:B38" xr:uid="{51C8EE75-88EB-44C3-B3DF-8EDD52F15786}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CE4556E8-E479-4C63-BA11-D7A281150AD9}" name="BenchBoards"/>
+    <tableColumn id="1" xr3:uid="{CE4556E8-E479-4C63-BA11-D7A281150AD9}" name="Annunciator"/>
     <tableColumn id="2" xr3:uid="{50F9665B-7BCF-4330-82AA-B3916D694ED7}" name="IP Address"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -845,7 +885,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FF5F106-0E09-4A99-A021-E84F5598FF4F}" name="Table4" displayName="Table4" ref="A40:B43" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FF5F106-0E09-4A99-A021-E84F5598FF4F}" name="Table4" displayName="Table4" ref="A40:B43" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A40:B43" xr:uid="{1FF5F106-0E09-4A99-A021-E84F5598FF4F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C7AC28FC-F22C-47DB-BFC1-EE01BC836B4D}" name="HMI"/>
@@ -856,7 +896,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D49AE364-6D28-4A79-B7DA-72A00A0F8E39}" name="Table5" displayName="Table5" ref="A1:E16" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D49AE364-6D28-4A79-B7DA-72A00A0F8E39}" name="Table5" displayName="Table5" ref="A1:E16" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A1:E16" xr:uid="{D49AE364-6D28-4A79-B7DA-72A00A0F8E39}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{6097A296-7764-40B4-B83C-4908FFF60966}" name="NUC Name">
@@ -872,10 +912,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9AA7F9D4-2F84-45A6-951D-F3D6DDF6E91E}" name="Table7" displayName="Table7" ref="A1:D10" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9AA7F9D4-2F84-45A6-951D-F3D6DDF6E91E}" name="Table7" displayName="Table7" ref="A1:D10" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A1:D10" xr:uid="{9AA7F9D4-2F84-45A6-951D-F3D6DDF6E91E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{98D2039C-6787-43B3-9114-D3169FE183CA}" name="NUC Name" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{98D2039C-6787-43B3-9114-D3169FE183CA}" name="NUC Name" dataDxfId="11">
       <calculatedColumnFormula>Master!A19</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{59235F5F-66E3-48A2-B11F-9A6219AF04AF}" name="1"/>
@@ -887,10 +927,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C7A265E5-1D21-469C-8C66-AE2DEAD0EF28}" name="Table8" displayName="Table8" ref="A1:F10" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C7A265E5-1D21-469C-8C66-AE2DEAD0EF28}" name="Table8" displayName="Table8" ref="A1:F10" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:F10" xr:uid="{C7A265E5-1D21-469C-8C66-AE2DEAD0EF28}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6DA18596-A12D-46AC-B647-CE603C9DA47B}" name="NUC Name" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{6DA18596-A12D-46AC-B647-CE603C9DA47B}" name="NUC Name" dataDxfId="7">
       <calculatedColumnFormula>Master!A30</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{F3D7C38D-59C7-4B65-8C9C-EFE9BFAB2355}" name="1"/>
@@ -904,10 +944,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C1130CA8-D1C4-41B7-B1A8-BED2E10241CD}" name="Table9" displayName="Table9" ref="A1:C4" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C1130CA8-D1C4-41B7-B1A8-BED2E10241CD}" name="Table9" displayName="Table9" ref="A1:C4" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:C4" xr:uid="{C1130CA8-D1C4-41B7-B1A8-BED2E10241CD}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AB27A4F2-A451-459B-AC97-3C7D8F223B8D}" name="NUC Name" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{AB27A4F2-A451-459B-AC97-3C7D8F223B8D}" name="NUC Name" dataDxfId="3">
       <calculatedColumnFormula>Master!A41</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{371F32D2-B54E-4E02-A0EA-0D617F82AAA8}" name="1"/>
@@ -919,7 +959,13 @@
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{291801C9-339D-4EF3-B305-0C3698772A70}" name="Table10" displayName="Table10" ref="A1:H37" totalsRowShown="0">
-  <autoFilter ref="A1:H37" xr:uid="{291801C9-339D-4EF3-B305-0C3698772A70}"/>
+  <autoFilter ref="A1:H37" xr:uid="{291801C9-339D-4EF3-B305-0C3698772A70}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9FDD98CA-67A7-4AB2-9FFA-422A8C49A11E}" name="NUC name"/>
     <tableColumn id="2" xr3:uid="{BE184B61-231C-4615-B5B7-03FDD1C24B7E}" name="1"/>
@@ -1200,7 +1246,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,7 +1465,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>3</v>
@@ -2334,7 +2380,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,106 +2417,106 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4" t="b">
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3" t="b">
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="b">
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="b">
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
         <v>0</v>
       </c>
       <c r="G5" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2496,7 +2542,7 @@
       <c r="G6" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2522,7 +2568,7 @@
       <c r="G7" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2548,7 +2594,7 @@
       <c r="G8" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2574,7 +2620,7 @@
       <c r="G9" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2600,7 +2646,7 @@
       <c r="G10" t="s">
         <v>92</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2670,7 +2716,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -2687,13 +2733,13 @@
         <v>43</v>
       </c>
       <c r="B14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -3002,10 +3048,10 @@
         <v>1</v>
       </c>
       <c r="C26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -3028,10 +3074,10 @@
         <v>1</v>
       </c>
       <c r="C27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -3054,10 +3100,10 @@
         <v>1</v>
       </c>
       <c r="C28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -3080,10 +3126,10 @@
         <v>1</v>
       </c>
       <c r="C29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -3106,10 +3152,10 @@
         <v>1</v>
       </c>
       <c r="C30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -3132,10 +3178,10 @@
         <v>1</v>
       </c>
       <c r="C31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -3158,10 +3204,10 @@
         <v>1</v>
       </c>
       <c r="C32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -3184,10 +3230,10 @@
         <v>1</v>
       </c>
       <c r="C33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -3210,10 +3256,10 @@
         <v>1</v>
       </c>
       <c r="C34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -3308,6 +3354,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A2:H37">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>